<commit_message>
Python script excel to db
</commit_message>
<xml_diff>
--- a/db-base-info.xlsx
+++ b/db-base-info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\OneDrive\Escritorio\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\OneDrive\Escritorio\D5\ost-videogames-covers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DE47F3-BC44-4100-9920-A4420243919A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7639BEFC-BE73-4528-AA09-E77B73B21AC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="699">
   <si>
     <t>id</t>
   </si>
@@ -1578,13 +1578,553 @@
   </si>
   <si>
     <t>https://vgmsite.com/soundtracks/donkey-kong-country/hhvtfdcu/02%20-%20Simian%20Segue.mp3</t>
+  </si>
+  <si>
+    <t>DK Island Swing</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country/zmyayhqp/04%20-%20DK%20Island%20Swing.mp3</t>
+  </si>
+  <si>
+    <t>Cranky's Theme</t>
+  </si>
+  <si>
+    <t>(01:17)</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country/itvsmvih/05%20-%20Cranky%27s%20Theme.mp3</t>
+  </si>
+  <si>
+    <t>(03:09)</t>
+  </si>
+  <si>
+    <t>Cave Dweller Concert</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country/pojkaorc/06%20-%20Cave%20Dweller%20Concert.mp3</t>
+  </si>
+  <si>
+    <t>Bonus Room Blitz</t>
+  </si>
+  <si>
+    <t>(00:59)</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country/oxspowyu/07%20-%20Bonus%20Room%20Blitz.mp3</t>
+  </si>
+  <si>
+    <t>Aquatic Ambiance</t>
+  </si>
+  <si>
+    <t>(03:26)</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country/ycexnxet/08%20-%20Aquatic%20Ambiance.mp3</t>
+  </si>
+  <si>
+    <t>Candy's Love Song</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country/qgrvzwsi/09%20-%20Candy%27s%20Love%20Song.mp3</t>
+  </si>
+  <si>
+    <t>Bad Boss Boogie</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country/psjstlgy/10%20-%20Bad%20Boss%20Boogie.mp3</t>
+  </si>
+  <si>
+    <t>Mine Cart Madness</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country/rwyezinz/11%20-%20Mine%20Cart%20Madness.mp3</t>
+  </si>
+  <si>
+    <t>Life in the Mines</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country/orvxlyep/12%20-%20Life%20in%20the%20Mines.mp3</t>
+  </si>
+  <si>
+    <t>Voices of the Temple</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country/njvnpzie/13%20-%20Voices%20of%20the%20Temple.mp3</t>
+  </si>
+  <si>
+    <t>Forest Frenzy</t>
+  </si>
+  <si>
+    <t>(02:02)</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country/cgmufbnb/14%20-%20Forest%20Frenzy.mp3</t>
+  </si>
+  <si>
+    <t>Treetop Rock</t>
+  </si>
+  <si>
+    <t>(01:58)</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country/bbtakkjy/15%20-%20Treetop%20Rock.mp3</t>
+  </si>
+  <si>
+    <t>Funky's Fugue</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country/bytbjjvs/16%20-%20Funky%27s%20Fugue.mp3</t>
+  </si>
+  <si>
+    <t>Misty Menace</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country/nvmacotf/17%20-%20Misty%20Menace.mp3</t>
+  </si>
+  <si>
+    <t>Northern Hemispheres</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country/bghrfsbm/18%20-%20Northern%20Hemispheres.mp3</t>
+  </si>
+  <si>
+    <t>Ice Cave Chant</t>
+  </si>
+  <si>
+    <t>(02:04)</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country/dzqzcyjy/19%20-%20Ice%20Cave%20Chant.mp3</t>
+  </si>
+  <si>
+    <t>Fear Factory</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country/pronvibn/20%20-%20Fear%20Factory.mp3</t>
+  </si>
+  <si>
+    <t>Gang-Plank Galleon</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country/mozqcjlc/21%20-%20Gang-Plank%20Galleon.mp3</t>
+  </si>
+  <si>
+    <t>K. Rool's Cacophony</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country/diayekwl/22%20-%20K.%20Rool%27s%20Cacophony.mp3</t>
+  </si>
+  <si>
+    <t>The Credits Concerto</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country/oexjynvg/23%20-%20The%20Credits%20Concerto.mp3</t>
+  </si>
+  <si>
+    <t>Stage Clear</t>
+  </si>
+  <si>
+    <t>(00:07)</t>
+  </si>
+  <si>
+    <t>Lose</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country/aypaecrt/24%20-%20Stage%20Clear.mp3</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country/wofnsjjf/25%20-%20Lose.mp3</t>
+  </si>
+  <si>
+    <t>Bonus Lose</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country/whkuqswr/26%20-%20Bonus%20Lose.mp3</t>
+  </si>
+  <si>
+    <t>Bonus Win</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country/mgekqeja/27%20-%20Bonus%20Win.mp3</t>
+  </si>
+  <si>
+    <t>Donkey Kong Country 2 - Diddy's Kong Quest</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/front.png</t>
+  </si>
+  <si>
+    <t>K. Rool Returns</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/knmbdkowch/01%20-%20K.%20Rool%20Returns.mp3</t>
+  </si>
+  <si>
+    <t>Welcome To Crocodile Isle</t>
+  </si>
+  <si>
+    <t>(01:13)</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/lowmkcyoxr/02%20-%20Welcome%20To%20Crocodile%20Isle.mp3</t>
+  </si>
+  <si>
+    <t>Klomp's Romp</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/ysuavweflp/03%20-%20Klomp%27s%20Romp.mp3</t>
+  </si>
+  <si>
+    <t>Lockjaw's Saga</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/xpcbunqdfx/04%20-%20Lockjaw%27s%20Saga.mp3</t>
+  </si>
+  <si>
+    <t>Jib Jig</t>
+  </si>
+  <si>
+    <t>(02:00)</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/eyzzjmoiqy/05%20-%20Jib%20Jig.mp3</t>
+  </si>
+  <si>
+    <t>Swanky Swing</t>
+  </si>
+  <si>
+    <t>(01:00)</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/nskrayfuws/06%20-%20Swanky%20Swing.mp3</t>
+  </si>
+  <si>
+    <t>Snakey Chantey</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/rchzqlcegm/07%20-%20Snakey%20Chantey.mp3</t>
+  </si>
+  <si>
+    <t>Bayou Boogie</t>
+  </si>
+  <si>
+    <t>(01:41)</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/jzdrvsfmwb/08%20-%20Bayou%20Boogie.mp3</t>
+  </si>
+  <si>
+    <t>School House Harmony</t>
+  </si>
+  <si>
+    <t>(01:49)</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/zkblkjyxlo/09%20-%20School%20House%20Harmony.mp3</t>
+  </si>
+  <si>
+    <t>Forest Interlude</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/krlpffkbsb/10%20-%20Forest%20Interlude.mp3</t>
+  </si>
+  <si>
+    <t>Funky The Main Monkey</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/wuiyxsbvue/11%20-%20Funky%20The%20Main%20Monkey.mp3</t>
+  </si>
+  <si>
+    <t>Flight of the Zinger</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/etwxcheifa/12%20-%20Flight%20of%20the%20Zinger.mp3</t>
+  </si>
+  <si>
+    <t>Cranky's Conga</t>
+  </si>
+  <si>
+    <t>(01:26)</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/fxnwpdllgb/13%20-%20Cranky%27s%20Conga.mp3</t>
+  </si>
+  <si>
+    <t>Hot-Head Bop</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/vzaufqcrix/14%20-%20Hot-Head%20Bop.mp3</t>
+  </si>
+  <si>
+    <t>Run, Rambi! Run!</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/dudkiuwtvs/15%20-%20Run%2C%20Rambi%21%20Run%21.mp3</t>
+  </si>
+  <si>
+    <t>Token Tango</t>
+  </si>
+  <si>
+    <t>(01:15)</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/dbzdgxzsyc/16%20-%20Token%20Tango.mp3</t>
+  </si>
+  <si>
+    <t>Stickerbush Symphony</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/lzxtfubavq/17%20-%20Stickerbush%20Symphony.mp3</t>
+  </si>
+  <si>
+    <t>Bad Bird Rag</t>
+  </si>
+  <si>
+    <t>(01:06)</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/vabarhzxml/18%20-%20Bad%20Bird%20Rag.mp3</t>
+  </si>
+  <si>
+    <t>Disco Train</t>
+  </si>
+  <si>
+    <t>(02:39)</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/nuytvwttth/19%20-%20Disco%20Train.mp3</t>
+  </si>
+  <si>
+    <t>Boss Bossanova</t>
+  </si>
+  <si>
+    <t>(01:16)</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/qgowlrjqww/20%20-%20Boss%20Bossanova.mp3</t>
+  </si>
+  <si>
+    <t>Steel Drum Rhumba</t>
+  </si>
+  <si>
+    <t>(01:08)</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/qyaftmgssn/21%20-%20Steel%20Drum%20Rhumba.mp3</t>
+  </si>
+  <si>
+    <t>Krook's March</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/opckakwxmb/22%20-%20Krook%27s%20March.mp3</t>
+  </si>
+  <si>
+    <t>Klubba's Reveille</t>
+  </si>
+  <si>
+    <t>(01:09)</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/xlatgwfgrs/23%20-%20Klubba%27s%20Reveille.mp3</t>
+  </si>
+  <si>
+    <t>Haunted Chase</t>
+  </si>
+  <si>
+    <t>(02:23)</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/yjrzhthifg/24%20-%20Haunted%20Chase.mp3</t>
+  </si>
+  <si>
+    <t>In A Snow-Bound Land</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/ryxmuhrfek/25%20-%20In%20A%20Snow-Bound%20Land.mp3</t>
+  </si>
+  <si>
+    <t>Lost World Anthem</t>
+  </si>
+  <si>
+    <t>(01:44)</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/apxosstakl/26%20-%20Lost%20World%20Anthem.mp3</t>
+  </si>
+  <si>
+    <t>Primal Rave</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/dpeeyuezjb/27%20-%20Primal%20Rave.mp3</t>
+  </si>
+  <si>
+    <t>Crocodile Cacophony</t>
+  </si>
+  <si>
+    <t>(01:33)</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/raffknzcxp/28%20-%20Crocodile%20Cacophony.mp3</t>
+  </si>
+  <si>
+    <t>Donkey Kong Rescued</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/xvrjputxcm/29%20-%20Donkey%20Kong%20Rescued.mp3</t>
+  </si>
+  <si>
+    <t>Rare Logo</t>
+  </si>
+  <si>
+    <t>(00:14)</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/kuqdgyopdk/35%20-%20Rare%20Logo.mp3</t>
+  </si>
+  <si>
+    <t>Failure 1</t>
+  </si>
+  <si>
+    <t>Failure 2</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/ypummzlhps/36%20-%20Failure%201.mp3</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/ztwkutatsc/37%20-%20Failure%202.mp3</t>
+  </si>
+  <si>
+    <t>Faulire 3</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/mwotusdwre/38%20-%20Faulire%203.mp3</t>
+  </si>
+  <si>
+    <t>Failure 4</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/tekukdgjij/39%20-%20Failure%204.mp3</t>
+  </si>
+  <si>
+    <t>Failure 5</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/cjstzofpgi/40%20-%20Failure%205.mp3</t>
+  </si>
+  <si>
+    <t>Failure 6</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/ljsglifrny/41%20-%20Failure%206.mp3</t>
+  </si>
+  <si>
+    <t>Failure 7</t>
+  </si>
+  <si>
+    <t>(00:15)</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/jmbbhaywak/42%20-%20Failure%207.mp3</t>
+  </si>
+  <si>
+    <t>Failure 8</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/hqntxqsuth/43%20-%20Failure%208.mp3</t>
+  </si>
+  <si>
+    <t>Failure 9</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/ztkuuwlcln/44%20-%20Failure%209.mp3</t>
+  </si>
+  <si>
+    <t>Failure 10</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/vvaxpaxnor/45%20-%20Failure%2010.mp3</t>
+  </si>
+  <si>
+    <t>Failure 11</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/zeqxutrrlg/46%20-%20Failure%2011.mp3</t>
+  </si>
+  <si>
+    <t>Failure 12</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/uewimcopmg/47%20-%20Failure%2012.mp3</t>
+  </si>
+  <si>
+    <t>Failure 13</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/xyhavtjgne/48%20-%20Failure%2013.mp3</t>
+  </si>
+  <si>
+    <t>Failure 14</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/lgorqdaunt/49%20-%20Failure%2014.mp3</t>
+  </si>
+  <si>
+    <t>Failure 15</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/tzfjdmijsp/50%20-%20Failure%2015.mp3</t>
+  </si>
+  <si>
+    <t>Failure 16</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/bftdeairjj/54%20-%20Failure%2016.mp3</t>
+  </si>
+  <si>
+    <t>Diddy's Victory</t>
+  </si>
+  <si>
+    <t>(00:27)</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/mlmwmavlqu/51%20-%20Diddy%27s%20Victory.mp3</t>
+  </si>
+  <si>
+    <t>Dixie's Victory</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/tngdbfmqve/52%20-%20Dixie%27s%20Victory.mp3</t>
+  </si>
+  <si>
+    <t>False Triumph</t>
+  </si>
+  <si>
+    <t>(00:37)</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/kufapmwpqv/53%20-%20False%20Triumph%20.mp3</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-02-diddys-kong-quest/zuihwijfqb/55%20-%20Game%20Over.mp3</t>
+  </si>
+  <si>
+    <t>Donkey Kong Country 3 - Dixie Kong's Double Trouble OST</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-3-dixie-kong-s-double-trouble-ost/front.jpg</t>
+  </si>
+  <si>
+    <t>Dixie Beat</t>
+  </si>
+  <si>
+    <t>https://vgmsite.com/soundtracks/donkey-kong-country-3-dixie-kong-s-double-trouble-ost/lrubqlgbqx/01%20-%20Dixie%20Beat.mp3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1625,6 +2165,32 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1643,20 +2209,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1870,16 +2446,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19884A20-ED99-4389-8ABD-58FFD81E92B6}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="56.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="90" bestFit="1" customWidth="1"/>
@@ -2068,8 +2644,42 @@
       <c r="D11" s="4" t="s">
         <v>509</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="5" t="s">
         <v>511</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>510</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>695</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="E13" t="s">
+        <v>696</v>
       </c>
     </row>
   </sheetData>
@@ -2083,23 +2693,25 @@
     <hyperlink ref="E8" r:id="rId7" xr:uid="{A45CB169-8EFD-4D8B-8637-4E657ABCEE64}"/>
     <hyperlink ref="E9" r:id="rId8" xr:uid="{8DBC3CFB-8533-4130-BA8D-2A5C245DFE1C}"/>
     <hyperlink ref="E10" r:id="rId9" xr:uid="{A30189B5-4F63-457E-B4A7-DE09EBCE74DE}"/>
+    <hyperlink ref="E12" r:id="rId10" xr:uid="{C250A1C3-2425-403E-AE0B-EDDF90B3448E}"/>
+    <hyperlink ref="E11" r:id="rId11" xr:uid="{3924E06E-AB8A-4369-AB48-282C1DA8E900}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF22B381-0806-4C04-BEA9-05569D6B53DA}">
-  <dimension ref="A1:D193"/>
+  <dimension ref="A1:D268"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
-      <selection activeCell="D196" sqref="B184:D196"/>
+      <selection activeCell="B278" sqref="B278"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="196.6640625" bestFit="1" customWidth="1"/>
@@ -4769,13 +5381,13 @@
       <c r="A191" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="B191" t="s">
+      <c r="B191" s="4" t="s">
         <v>512</v>
       </c>
       <c r="C191" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D191" s="6" t="s">
         <v>514</v>
       </c>
     </row>
@@ -4783,13 +5395,13 @@
       <c r="A192" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="B192" s="5" t="s">
+      <c r="B192" s="8" t="s">
         <v>516</v>
       </c>
       <c r="C192" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D192" t="s">
+      <c r="D192" s="4" t="s">
         <v>517</v>
       </c>
     </row>
@@ -4803,8 +5415,1058 @@
       <c r="C193" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D193" s="4" t="s">
         <v>518</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A194" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="B194" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="C194" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D194" s="6" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A195" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="B195" s="9" t="s">
+        <v>521</v>
+      </c>
+      <c r="C195" s="4" t="s">
+        <v>522</v>
+      </c>
+      <c r="D195" s="5" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A196" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="B196" s="9" t="s">
+        <v>525</v>
+      </c>
+      <c r="C196" s="4" t="s">
+        <v>524</v>
+      </c>
+      <c r="D196" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A197" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="B197" s="9" t="s">
+        <v>527</v>
+      </c>
+      <c r="C197" s="4" t="s">
+        <v>528</v>
+      </c>
+      <c r="D197" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A198" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="B198" s="9" t="s">
+        <v>530</v>
+      </c>
+      <c r="C198" s="4" t="s">
+        <v>531</v>
+      </c>
+      <c r="D198" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A199" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="B199" s="9" t="s">
+        <v>533</v>
+      </c>
+      <c r="C199" s="4" t="s">
+        <v>522</v>
+      </c>
+      <c r="D199" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A200" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="B200" s="9" t="s">
+        <v>535</v>
+      </c>
+      <c r="C200" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D200" s="5" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A201" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="B201" s="9" t="s">
+        <v>537</v>
+      </c>
+      <c r="C201" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D201" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A202" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="B202" s="9" t="s">
+        <v>539</v>
+      </c>
+      <c r="C202" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D202" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A203" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="B203" s="9" t="s">
+        <v>541</v>
+      </c>
+      <c r="C203" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="D203" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A204" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="B204" s="9" t="s">
+        <v>543</v>
+      </c>
+      <c r="C204" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="D204" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A205" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="B205" s="9" t="s">
+        <v>546</v>
+      </c>
+      <c r="C205" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="D205" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A206" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="B206" s="9" t="s">
+        <v>549</v>
+      </c>
+      <c r="C206" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D206" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A207" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="B207" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="C207" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D207" s="5" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A208" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="B208" s="9" t="s">
+        <v>553</v>
+      </c>
+      <c r="C208" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="D208" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A209" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="B209" s="9" t="s">
+        <v>555</v>
+      </c>
+      <c r="C209" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="D209" s="5" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A210" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="B210" s="9" t="s">
+        <v>558</v>
+      </c>
+      <c r="C210" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D210" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A211" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="B211" s="9" t="s">
+        <v>560</v>
+      </c>
+      <c r="C211" s="4" t="s">
+        <v>485</v>
+      </c>
+      <c r="D211" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A212" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="B212" s="9" t="s">
+        <v>562</v>
+      </c>
+      <c r="C212" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D212" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A213" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="B213" s="9" t="s">
+        <v>564</v>
+      </c>
+      <c r="C213" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D213" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A214" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="B214" s="9" t="s">
+        <v>566</v>
+      </c>
+      <c r="C214" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="D214" s="5" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A215" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="B215" s="9" t="s">
+        <v>568</v>
+      </c>
+      <c r="C215" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D215" s="5" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A216" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="B216" s="9" t="s">
+        <v>571</v>
+      </c>
+      <c r="C216" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D216" s="5" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A217" s="7" t="s">
+        <v>509</v>
+      </c>
+      <c r="B217" s="9" t="s">
+        <v>573</v>
+      </c>
+      <c r="C217" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D217" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A218" s="9" t="s">
+        <v>575</v>
+      </c>
+      <c r="B218" s="10" t="s">
+        <v>577</v>
+      </c>
+      <c r="C218" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D218" s="5" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A219" s="9" t="s">
+        <v>575</v>
+      </c>
+      <c r="B219" s="10" t="s">
+        <v>579</v>
+      </c>
+      <c r="C219" s="4" t="s">
+        <v>580</v>
+      </c>
+      <c r="D219" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A220" s="9" t="s">
+        <v>575</v>
+      </c>
+      <c r="B220" s="10" t="s">
+        <v>582</v>
+      </c>
+      <c r="C220" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="D220" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A221" t="s">
+        <v>575</v>
+      </c>
+      <c r="B221" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="C221" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D221" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
+        <v>575</v>
+      </c>
+      <c r="B222" s="10" t="s">
+        <v>586</v>
+      </c>
+      <c r="C222" s="4" t="s">
+        <v>587</v>
+      </c>
+      <c r="D222" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A223" t="s">
+        <v>575</v>
+      </c>
+      <c r="B223" s="10" t="s">
+        <v>589</v>
+      </c>
+      <c r="C223" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="D223" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
+        <v>575</v>
+      </c>
+      <c r="B224" s="10" t="s">
+        <v>592</v>
+      </c>
+      <c r="C224" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="D224" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
+        <v>575</v>
+      </c>
+      <c r="B225" s="10" t="s">
+        <v>594</v>
+      </c>
+      <c r="C225" s="4" t="s">
+        <v>595</v>
+      </c>
+      <c r="D225" s="5" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>575</v>
+      </c>
+      <c r="B226" s="10" t="s">
+        <v>597</v>
+      </c>
+      <c r="C226" s="4" t="s">
+        <v>598</v>
+      </c>
+      <c r="D226" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
+        <v>575</v>
+      </c>
+      <c r="B227" s="10" t="s">
+        <v>600</v>
+      </c>
+      <c r="C227" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="D227" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
+        <v>575</v>
+      </c>
+      <c r="B228" s="10" t="s">
+        <v>602</v>
+      </c>
+      <c r="C228" s="4" t="s">
+        <v>492</v>
+      </c>
+      <c r="D228" s="5" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
+        <v>575</v>
+      </c>
+      <c r="B229" s="10" t="s">
+        <v>604</v>
+      </c>
+      <c r="C229" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D229" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
+        <v>575</v>
+      </c>
+      <c r="B230" s="9" t="s">
+        <v>606</v>
+      </c>
+      <c r="C230" s="4" t="s">
+        <v>607</v>
+      </c>
+      <c r="D230" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
+        <v>575</v>
+      </c>
+      <c r="B231" s="9" t="s">
+        <v>609</v>
+      </c>
+      <c r="C231" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D231" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
+        <v>575</v>
+      </c>
+      <c r="B232" s="9" t="s">
+        <v>611</v>
+      </c>
+      <c r="C232" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="D232" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A233" t="s">
+        <v>575</v>
+      </c>
+      <c r="B233" s="9" t="s">
+        <v>613</v>
+      </c>
+      <c r="C233" s="4" t="s">
+        <v>614</v>
+      </c>
+      <c r="D233" s="5" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
+        <v>575</v>
+      </c>
+      <c r="B234" s="9" t="s">
+        <v>616</v>
+      </c>
+      <c r="C234" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="D234" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A235" t="s">
+        <v>575</v>
+      </c>
+      <c r="B235" s="9" t="s">
+        <v>618</v>
+      </c>
+      <c r="C235" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="D235" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A236" t="s">
+        <v>575</v>
+      </c>
+      <c r="B236" s="9" t="s">
+        <v>621</v>
+      </c>
+      <c r="C236" s="4" t="s">
+        <v>622</v>
+      </c>
+      <c r="D236" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A237" t="s">
+        <v>575</v>
+      </c>
+      <c r="B237" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="C237" s="4" t="s">
+        <v>625</v>
+      </c>
+      <c r="D237" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A238" t="s">
+        <v>575</v>
+      </c>
+      <c r="B238" s="9" t="s">
+        <v>627</v>
+      </c>
+      <c r="C238" s="4" t="s">
+        <v>628</v>
+      </c>
+      <c r="D238" s="5" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A239" t="s">
+        <v>575</v>
+      </c>
+      <c r="B239" s="9" t="s">
+        <v>630</v>
+      </c>
+      <c r="C239" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="D239" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A240" t="s">
+        <v>575</v>
+      </c>
+      <c r="B240" s="9" t="s">
+        <v>632</v>
+      </c>
+      <c r="C240" s="4" t="s">
+        <v>633</v>
+      </c>
+      <c r="D240" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A241" t="s">
+        <v>575</v>
+      </c>
+      <c r="B241" s="9" t="s">
+        <v>635</v>
+      </c>
+      <c r="C241" s="4" t="s">
+        <v>636</v>
+      </c>
+      <c r="D241" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A242" t="s">
+        <v>575</v>
+      </c>
+      <c r="B242" s="9" t="s">
+        <v>638</v>
+      </c>
+      <c r="C242" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D242" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A243" s="7" t="s">
+        <v>575</v>
+      </c>
+      <c r="B243" s="9" t="s">
+        <v>640</v>
+      </c>
+      <c r="C243" s="4" t="s">
+        <v>641</v>
+      </c>
+      <c r="D243" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A244" t="s">
+        <v>575</v>
+      </c>
+      <c r="B244" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="C244" s="4" t="s">
+        <v>485</v>
+      </c>
+      <c r="D244" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A245" t="s">
+        <v>575</v>
+      </c>
+      <c r="B245" s="9" t="s">
+        <v>645</v>
+      </c>
+      <c r="C245" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="D245" s="5" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A246" t="s">
+        <v>575</v>
+      </c>
+      <c r="B246" s="9" t="s">
+        <v>648</v>
+      </c>
+      <c r="C246" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D246" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A247" t="s">
+        <v>575</v>
+      </c>
+      <c r="B247" s="9" t="s">
+        <v>650</v>
+      </c>
+      <c r="C247" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="D247" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A248" t="s">
+        <v>575</v>
+      </c>
+      <c r="B248" s="9" t="s">
+        <v>653</v>
+      </c>
+      <c r="C248" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="D248" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A249" t="s">
+        <v>575</v>
+      </c>
+      <c r="B249" s="10" t="s">
+        <v>654</v>
+      </c>
+      <c r="C249" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D249" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A250" t="s">
+        <v>575</v>
+      </c>
+      <c r="B250" s="10" t="s">
+        <v>657</v>
+      </c>
+      <c r="C250" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D250" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A251" t="s">
+        <v>575</v>
+      </c>
+      <c r="B251" s="10" t="s">
+        <v>659</v>
+      </c>
+      <c r="C251" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="D251" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A252" t="s">
+        <v>575</v>
+      </c>
+      <c r="B252" s="10" t="s">
+        <v>661</v>
+      </c>
+      <c r="C252" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="D252" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A253" t="s">
+        <v>575</v>
+      </c>
+      <c r="B253" s="10" t="s">
+        <v>663</v>
+      </c>
+      <c r="C253" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="D253" s="5" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A254" t="s">
+        <v>575</v>
+      </c>
+      <c r="B254" s="10" t="s">
+        <v>665</v>
+      </c>
+      <c r="C254" s="4" t="s">
+        <v>666</v>
+      </c>
+      <c r="D254" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A255" t="s">
+        <v>575</v>
+      </c>
+      <c r="B255" s="10" t="s">
+        <v>668</v>
+      </c>
+      <c r="C255" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D255" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A256" t="s">
+        <v>575</v>
+      </c>
+      <c r="B256" s="10" t="s">
+        <v>670</v>
+      </c>
+      <c r="C256" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D256" s="5" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A257" t="s">
+        <v>575</v>
+      </c>
+      <c r="B257" s="10" t="s">
+        <v>672</v>
+      </c>
+      <c r="C257" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D257" s="5" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A258" t="s">
+        <v>575</v>
+      </c>
+      <c r="B258" s="10" t="s">
+        <v>674</v>
+      </c>
+      <c r="C258" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D258" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A259" t="s">
+        <v>575</v>
+      </c>
+      <c r="B259" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="C259" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D259" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A260" t="s">
+        <v>575</v>
+      </c>
+      <c r="B260" s="10" t="s">
+        <v>678</v>
+      </c>
+      <c r="C260" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="D260" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A261" t="s">
+        <v>575</v>
+      </c>
+      <c r="B261" s="10" t="s">
+        <v>680</v>
+      </c>
+      <c r="C261" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D261" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A262" t="s">
+        <v>575</v>
+      </c>
+      <c r="B262" s="10" t="s">
+        <v>682</v>
+      </c>
+      <c r="C262" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D262" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A263" t="s">
+        <v>575</v>
+      </c>
+      <c r="B263" s="10" t="s">
+        <v>684</v>
+      </c>
+      <c r="C263" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D263" s="5" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A264" t="s">
+        <v>575</v>
+      </c>
+      <c r="B264" s="10" t="s">
+        <v>686</v>
+      </c>
+      <c r="C264" s="4" t="s">
+        <v>687</v>
+      </c>
+      <c r="D264" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A265" t="s">
+        <v>575</v>
+      </c>
+      <c r="B265" s="10" t="s">
+        <v>689</v>
+      </c>
+      <c r="C265" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="D265" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A266" t="s">
+        <v>575</v>
+      </c>
+      <c r="B266" s="10" t="s">
+        <v>691</v>
+      </c>
+      <c r="C266" s="4" t="s">
+        <v>692</v>
+      </c>
+      <c r="D266" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A267" t="s">
+        <v>575</v>
+      </c>
+      <c r="B267" s="10" t="s">
+        <v>502</v>
+      </c>
+      <c r="C267" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="D267" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A268" t="s">
+        <v>695</v>
+      </c>
+      <c r="B268" s="9" t="s">
+        <v>697</v>
+      </c>
+      <c r="C268" s="4" t="s">
+        <v>595</v>
+      </c>
+      <c r="D268" t="s">
+        <v>698</v>
       </c>
     </row>
   </sheetData>
@@ -4999,7 +6661,27 @@
     <hyperlink ref="D188" r:id="rId187" xr:uid="{C1EA056F-78D3-47FA-ABC5-E5CD581F1683}"/>
     <hyperlink ref="D189" r:id="rId188" xr:uid="{346EB560-1598-408F-AAE8-2B60E61B7121}"/>
     <hyperlink ref="D190" r:id="rId189" xr:uid="{A0C656B3-43B0-4D5F-83CD-A42809CDDF8A}"/>
+    <hyperlink ref="D191" r:id="rId190" xr:uid="{9F4C611F-0A0B-42CA-9DE2-9F4366277BEB}"/>
+    <hyperlink ref="D194" r:id="rId191" xr:uid="{2BC27138-E867-42BC-8A16-C05625C3BCC4}"/>
+    <hyperlink ref="D195" r:id="rId192" xr:uid="{966F234C-C879-4AE7-B14D-EBEF5493ED73}"/>
+    <hyperlink ref="D200" r:id="rId193" xr:uid="{2BE18618-5014-4D69-9F7D-004C7EB94ED8}"/>
+    <hyperlink ref="D207" r:id="rId194" xr:uid="{6C6D018C-5524-46B5-9F2B-F0044881F741}"/>
+    <hyperlink ref="D209" r:id="rId195" xr:uid="{7A4C4AF9-FE2D-4E36-8CE9-5E46E381315C}"/>
+    <hyperlink ref="D214" r:id="rId196" xr:uid="{990CCF19-8B89-46D0-A518-90E4D8A3E843}"/>
+    <hyperlink ref="D215" r:id="rId197" xr:uid="{E32E9849-7F14-443D-AE05-6A98CFB5F956}"/>
+    <hyperlink ref="D216" r:id="rId198" xr:uid="{BDD17AD4-24D1-41B9-81DE-AEB275E442DC}"/>
+    <hyperlink ref="D228" r:id="rId199" xr:uid="{AD6E5442-E9E6-43B0-8A1A-C20F55E9563B}"/>
+    <hyperlink ref="D225" r:id="rId200" xr:uid="{E9868479-4F29-4891-BEC0-CD08B5E62D21}"/>
+    <hyperlink ref="D218" r:id="rId201" xr:uid="{3A485077-DD3C-4449-9445-ABE39509AA0B}"/>
+    <hyperlink ref="D233" r:id="rId202" xr:uid="{DE25AD8C-E6F8-4F15-844F-A149AE2966EC}"/>
+    <hyperlink ref="D238" r:id="rId203" xr:uid="{F4AA474E-15AF-4D61-856F-AE3091277A24}"/>
+    <hyperlink ref="D245" r:id="rId204" xr:uid="{422C48A6-ABA9-421E-A3C9-83AB22F446B1}"/>
+    <hyperlink ref="D253" r:id="rId205" xr:uid="{8D5BB15D-7F8D-428E-8878-5A95E7D4264A}"/>
+    <hyperlink ref="D256" r:id="rId206" xr:uid="{B8A138BF-63D2-4206-94EE-F97537B6AABF}"/>
+    <hyperlink ref="D257" r:id="rId207" xr:uid="{B1DF3083-24EE-4427-8D65-8760D2E6EB24}"/>
+    <hyperlink ref="D263" r:id="rId208" xr:uid="{123563BE-3D60-4318-8774-020701DAD9F3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId209"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix python insertion and correlative vg field
</commit_message>
<xml_diff>
--- a/db-base-info.xlsx
+++ b/db-base-info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/de71873dcf0b27a3/Escritorio/D5/CoverOST/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{7639BEFC-BE73-4528-AA09-E77B73B21AC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9A7ACA3D-6C14-4350-9366-0881583AC081}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{7639BEFC-BE73-4528-AA09-E77B73B21AC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{38F01A14-FD9B-412E-9081-93C594A83CBE}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="699">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="700">
   <si>
     <t>id</t>
   </si>
@@ -2118,6 +2118,9 @@
   </si>
   <si>
     <t>https://raw.githubusercontent.com/chelosky/ost-videogames-covers/main/covers/Donkey_Kong_Country3.jpg</t>
+  </si>
+  <si>
+    <t>correlative</t>
   </si>
 </sst>
 </file>
@@ -2442,11 +2445,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19884A20-ED99-4389-8ABD-58FFD81E92B6}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2454,10 +2455,11 @@
     <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="56.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="90" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="90" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2471,10 +2473,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>699</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2487,11 +2492,14 @@
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2504,11 +2512,14 @@
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2521,11 +2532,14 @@
       <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2538,11 +2552,14 @@
       <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2555,11 +2572,14 @@
       <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2572,11 +2592,14 @@
       <c r="D7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2">
+        <v>6</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2589,11 +2612,14 @@
       <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2">
+        <v>7</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2606,11 +2632,14 @@
       <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2">
+        <v>8</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2623,11 +2652,14 @@
       <c r="D10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2">
+        <v>9</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2640,11 +2672,14 @@
       <c r="D11" s="4" t="s">
         <v>509</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2657,11 +2692,14 @@
       <c r="D12" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="2">
+        <v>2</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -2674,24 +2712,27 @@
       <c r="D13" s="4" t="s">
         <v>509</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4">
+        <v>3</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>698</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{72D973CA-52F2-447E-A06A-AEA790FB587A}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{892CA4F7-625C-4C96-8210-CF6C60DB7E15}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{17258D48-DD72-43E2-841D-80947A69F27F}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{3A5526CD-652B-4D3D-939C-3B1C9A720949}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{79CEE65B-445F-4133-AD7A-74FBBDE604AF}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{649F0EC9-A574-43DD-B8FB-E18DAAD4A088}"/>
-    <hyperlink ref="E8" r:id="rId7" xr:uid="{A45CB169-8EFD-4D8B-8637-4E657ABCEE64}"/>
-    <hyperlink ref="E9" r:id="rId8" xr:uid="{8DBC3CFB-8533-4130-BA8D-2A5C245DFE1C}"/>
-    <hyperlink ref="E10" r:id="rId9" xr:uid="{A30189B5-4F63-457E-B4A7-DE09EBCE74DE}"/>
-    <hyperlink ref="E11" r:id="rId10" xr:uid="{3924E06E-AB8A-4369-AB48-282C1DA8E900}"/>
-    <hyperlink ref="E13" r:id="rId11" xr:uid="{CD953958-E07C-4CEE-8C0E-21A362A0E0FA}"/>
-    <hyperlink ref="E12" r:id="rId12" xr:uid="{015FA0AB-C1E7-4209-8CB4-3317322C3596}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{72D973CA-52F2-447E-A06A-AEA790FB587A}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{892CA4F7-625C-4C96-8210-CF6C60DB7E15}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{17258D48-DD72-43E2-841D-80947A69F27F}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{3A5526CD-652B-4D3D-939C-3B1C9A720949}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{79CEE65B-445F-4133-AD7A-74FBBDE604AF}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{649F0EC9-A574-43DD-B8FB-E18DAAD4A088}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{A45CB169-8EFD-4D8B-8637-4E657ABCEE64}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{8DBC3CFB-8533-4130-BA8D-2A5C245DFE1C}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{A30189B5-4F63-457E-B4A7-DE09EBCE74DE}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{3924E06E-AB8A-4369-AB48-282C1DA8E900}"/>
+    <hyperlink ref="F13" r:id="rId11" xr:uid="{CD953958-E07C-4CEE-8C0E-21A362A0E0FA}"/>
+    <hyperlink ref="F12" r:id="rId12" xr:uid="{015FA0AB-C1E7-4209-8CB4-3317322C3596}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>

</xml_diff>